<commit_message>
Added fuel technology Uranium
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_ELC_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_ELC_Techs.xlsx
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0">
+    <comment ref="F21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0">
+    <comment ref="G21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0">
+    <comment ref="H21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0">
+    <comment ref="I21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G28" authorId="0" shapeId="0">
+    <comment ref="G29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -475,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I28" authorId="0" shapeId="0">
+    <comment ref="I29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -775,7 +775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1072,6 +1072,21 @@
   </si>
   <si>
     <t>Kg/GJ</t>
+  </si>
+  <si>
+    <t>Fuel Technology Uranium ELC</t>
+  </si>
+  <si>
+    <t>FT-ELCURN</t>
+  </si>
+  <si>
+    <t>URN</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>PJa</t>
   </si>
 </sst>
 </file>
@@ -1773,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V44"/>
+  <dimension ref="B2:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2266,95 +2281,109 @@
       <c r="R16" s="28"/>
       <c r="S16" s="28"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16">
+        <v>1</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I21" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+    <row r="22" spans="2:19" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>70</v>
@@ -2364,109 +2393,101 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I29" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10" t="s">
+    <row r="30" spans="2:19" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I30" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="11" t="str">
+      <c r="C31" s="11" t="str">
         <f>B10</f>
         <v>ETURNLWR13N</v>
       </c>
-      <c r="D30" s="11" t="str">
+      <c r="D31" s="11" t="str">
         <f>C10</f>
         <v>Thermal electric: Nuclear plant LWR (III Gen.) - Average size</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="11" t="str">
-        <f>B15</f>
-        <v>ECNGAGTBP15N</v>
-      </c>
-      <c r="D31" s="11" t="str">
-        <f>C15</f>
-        <v xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </v>
       </c>
       <c r="E31" s="11" t="s">
         <v>70</v>
@@ -2480,91 +2501,127 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="11" t="str">
+        <f>B15</f>
+        <v>ECNGAGTBP15N</v>
+      </c>
+      <c r="D32" s="11" t="str">
+        <f>C15</f>
+        <v xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-    </row>
-    <row r="35" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+      <c r="I32" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="11" t="str">
+        <f>B17</f>
+        <v>FT-ELCURN</v>
+      </c>
+      <c r="D33" s="11" t="str">
+        <f>C17</f>
+        <v>Fuel Technology Uranium ELC</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="36" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+      <c r="C36" s="12"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C37" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="15" t="s">
+    <row r="38" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C38" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="16" t="s">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C39" s="16">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="5" t="s">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="13" t="s">
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C43" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D43" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="15" t="s">
+    <row r="44" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
I removed the FT for uranium
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_ELC_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_ELC_Techs.xlsx
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0">
+    <comment ref="F20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H21" authorId="0" shapeId="0">
+    <comment ref="H20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="0" shapeId="0">
+    <comment ref="I20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G29" authorId="0" shapeId="0">
+    <comment ref="G28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -475,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I29" authorId="0" shapeId="0">
+    <comment ref="I28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
+    <comment ref="B29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -775,7 +775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1072,21 +1072,6 @@
   </si>
   <si>
     <t>Kg/GJ</t>
-  </si>
-  <si>
-    <t>Fuel Technology Uranium ELC</t>
-  </si>
-  <si>
-    <t>FT-ELCURN</t>
-  </si>
-  <si>
-    <t>URN</t>
-  </si>
-  <si>
-    <t>PRE</t>
-  </si>
-  <si>
-    <t>PJa</t>
   </si>
 </sst>
 </file>
@@ -1788,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V45"/>
+  <dimension ref="B2:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2281,109 +2266,95 @@
       <c r="R16" s="28"/>
       <c r="S16" s="28"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="16" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16">
-        <v>1</v>
-      </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>67</v>
-      </c>
+      <c r="D22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>70</v>
@@ -2393,101 +2364,109 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
-      <c r="C24" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I28" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10" t="s">
+    <row r="29" spans="2:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F29" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="11" t="str">
+      <c r="C30" s="11" t="str">
         <f>B10</f>
         <v>ETURNLWR13N</v>
       </c>
-      <c r="D31" s="11" t="str">
+      <c r="D30" s="11" t="str">
         <f>C10</f>
         <v>Thermal electric: Nuclear plant LWR (III Gen.) - Average size</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="11" t="str">
+        <f>B15</f>
+        <v>ECNGAGTBP15N</v>
+      </c>
+      <c r="D31" s="11" t="str">
+        <f>C15</f>
+        <v xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </v>
       </c>
       <c r="E31" s="11" t="s">
         <v>70</v>
@@ -2501,127 +2480,81 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="11" t="str">
-        <f>B15</f>
-        <v>ECNGAGTBP15N</v>
-      </c>
-      <c r="D32" s="11" t="str">
-        <f>C15</f>
-        <v xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="11" t="str">
-        <f>B17</f>
-        <v>FT-ELCURN</v>
-      </c>
-      <c r="D33" s="11" t="str">
-        <f>C17</f>
-        <v>Fuel Technology Uranium ELC</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="36" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
+      <c r="C34" s="12"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C35" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="15" t="s">
+    <row r="36" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C36" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="16" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C37" s="16">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D41" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="15" t="s">
+    <row r="42" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
CHPR~FX changed into NCAP_CHPR
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_ELC_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_ELC_Techs.xlsx
@@ -1044,9 +1044,6 @@
     <t>M€/PJ</t>
   </si>
   <si>
-    <t>CHPR~FX</t>
-  </si>
-  <si>
     <t>Lead Time between investment decision and actual availability of capacity (equal to construction time)</t>
   </si>
   <si>
@@ -1072,6 +1069,9 @@
   </si>
   <si>
     <t>Kg/GJ</t>
+  </si>
+  <si>
+    <t>NCAP_CHPR</t>
   </si>
 </sst>
 </file>
@@ -1776,7 +1776,7 @@
   <dimension ref="B2:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1790,7 +1790,7 @@
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="7.109375" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
     <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.88671875" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
@@ -1864,7 +1864,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>57</v>
@@ -1888,10 +1888,10 @@
         <v>58</v>
       </c>
       <c r="R7" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="S7" s="17" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:22" s="3" customFormat="1" ht="38.700000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1920,7 +1920,7 @@
         <v>64</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>44</v>
@@ -1944,10 +1944,10 @@
         <v>45</v>
       </c>
       <c r="R8" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="S8" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="S8" s="18" t="s">
-        <v>91</v>
       </c>
       <c r="U8"/>
       <c r="V8"/>
@@ -1997,7 +1997,7 @@
         <v>74</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>68</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="15" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>84</v>
@@ -2502,12 +2502,12 @@
         <v>39</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="16">
         <v>57</v>

</xml_diff>

<commit_message>
Make compatible with Veda 2.0
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_ELC_Techs.xlsx
+++ b/SubRES_TMPL/SubRES_ELC_Techs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE65E75-074F-4824-A981-629C231E335F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="1368" windowWidth="17940" windowHeight="9852"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_Techs" sheetId="6" r:id="rId1"/>
@@ -15,17 +16,30 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -296,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -349,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0">
+    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -382,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G28" authorId="0" shapeId="0">
+    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -475,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I28" authorId="0" shapeId="0">
+    <comment ref="I28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -538,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -775,7 +789,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>~FI_T</t>
   </si>
@@ -783,301 +797,304 @@
     <t>TechName</t>
   </si>
   <si>
+    <t>Comm-IN</t>
+  </si>
+  <si>
+    <t>Comm-OUT</t>
+  </si>
+  <si>
+    <t>CommName</t>
+  </si>
+  <si>
+    <t>~FI_Comm</t>
+  </si>
+  <si>
+    <t>Csets</t>
+  </si>
+  <si>
+    <t>CommDesc</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>LimType</t>
+  </si>
+  <si>
+    <t>CTSLvl</t>
+  </si>
+  <si>
+    <t>PeakTS</t>
+  </si>
+  <si>
+    <t>Ctype</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>EFF</t>
+  </si>
+  <si>
+    <t>~COMEMI</t>
+  </si>
+  <si>
+    <t>~FI_Process</t>
+  </si>
+  <si>
+    <t>Tact</t>
+  </si>
+  <si>
+    <t>Tcap</t>
+  </si>
+  <si>
+    <t>Tslvl</t>
+  </si>
+  <si>
+    <t>PrimaryCG</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>\I: Commodity Set Membership</t>
+  </si>
+  <si>
+    <t>Commodity Name</t>
+  </si>
+  <si>
+    <t>Commodity Description</t>
+  </si>
+  <si>
+    <t>Balance Equ Type Override</t>
+  </si>
+  <si>
+    <t>Timeslice Tracking Level</t>
+  </si>
+  <si>
+    <t>Peak Monitoring</t>
+  </si>
+  <si>
+    <t>Electricity Indicator</t>
+  </si>
+  <si>
+    <t>\I: Process Set Membership</t>
+  </si>
+  <si>
+    <t>Technology Name</t>
+  </si>
+  <si>
+    <t>Technology Description</t>
+  </si>
+  <si>
+    <t>Activity Unit</t>
+  </si>
+  <si>
+    <t>Capacity Unit</t>
+  </si>
+  <si>
+    <t>Timeslice Operational Level</t>
+  </si>
+  <si>
+    <t>Operational Commodity Group</t>
+  </si>
+  <si>
+    <t>Vintage Tracking</t>
+  </si>
+  <si>
+    <t>&lt;Fuel Name&gt;</t>
+  </si>
+  <si>
+    <t>\I:Units</t>
+  </si>
+  <si>
+    <t>\I:Technology Name</t>
+  </si>
+  <si>
+    <t>Input Commodity</t>
+  </si>
+  <si>
+    <t>Output Commodity</t>
+  </si>
+  <si>
+    <t>Annual Availability Factor</t>
+  </si>
+  <si>
+    <t>Lifetime of Process</t>
+  </si>
+  <si>
+    <t>Capacity to Activity Factor</t>
+  </si>
+  <si>
+    <t>Starting Year</t>
+  </si>
+  <si>
+    <t>Investment Cost</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M Cost</t>
+  </si>
+  <si>
+    <t>Variable O&amp;M Cost</t>
+  </si>
+  <si>
+    <t>New Processes</t>
+  </si>
+  <si>
+    <t>*Declare and characterize the new technologies by sector. Sheet names should indicate the sector as &lt;SectorName&gt;_&lt;Anything&gt;</t>
+  </si>
+  <si>
+    <t>CURR</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Availabity/Utilization Factor</t>
+  </si>
+  <si>
+    <t>NCAP_TLIFE</t>
+  </si>
+  <si>
+    <t>PRC_CAPACT</t>
+  </si>
+  <si>
+    <t>NCAP_AFA</t>
+  </si>
+  <si>
+    <t>NCAP_AF</t>
+  </si>
+  <si>
+    <t>NCAP_FOM</t>
+  </si>
+  <si>
+    <t>ACT_COST</t>
+  </si>
+  <si>
+    <t>NCAP_COST</t>
+  </si>
+  <si>
+    <t>Technical Efficiency</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>~PRCCOMEMI</t>
+  </si>
+  <si>
+    <t>NRG</t>
+  </si>
+  <si>
+    <t>ELCURN</t>
+  </si>
+  <si>
+    <t>Uranium ELC</t>
+  </si>
+  <si>
+    <t>PJ</t>
+  </si>
+  <si>
+    <t>ELCNGA</t>
+  </si>
+  <si>
+    <t>Natural Gas ELC</t>
+  </si>
+  <si>
+    <t>ELE</t>
+  </si>
+  <si>
+    <t>ETURNLWR13N</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>*Unit</t>
+  </si>
+  <si>
+    <t>Currency unit</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>MEUR2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </t>
+  </si>
+  <si>
+    <t>MEUR2011</t>
+  </si>
+  <si>
+    <t>HET</t>
+  </si>
+  <si>
+    <t>M€/MW</t>
+  </si>
+  <si>
+    <t>M€/PJ</t>
+  </si>
+  <si>
+    <t>Lead Time between investment decision and actual availability of capacity (equal to construction time)</t>
+  </si>
+  <si>
+    <t>Fraction of capacity in peak equations</t>
+  </si>
+  <si>
+    <t>1/Cb: Ratio of heat produced to electricity produced</t>
+  </si>
+  <si>
+    <t>NCAP_ILED</t>
+  </si>
+  <si>
+    <t>NCAP_PKCNT</t>
+  </si>
+  <si>
+    <t>ECNGAGTBP15N</t>
+  </si>
+  <si>
+    <t>Thermal electric: Nuclear plant LWR (III Gen.) - Average size</t>
+  </si>
+  <si>
+    <t>ELCCO2</t>
+  </si>
+  <si>
+    <t>Kg/GJ</t>
+  </si>
+  <si>
+    <t>NCAP_CHPR</t>
+  </si>
+  <si>
+    <t>*TechDesc</t>
+  </si>
+  <si>
     <t>TechDesc</t>
-  </si>
-  <si>
-    <t>Comm-IN</t>
-  </si>
-  <si>
-    <t>Comm-OUT</t>
-  </si>
-  <si>
-    <t>CommName</t>
-  </si>
-  <si>
-    <t>~FI_Comm</t>
-  </si>
-  <si>
-    <t>Csets</t>
-  </si>
-  <si>
-    <t>CommDesc</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>LimType</t>
-  </si>
-  <si>
-    <t>CTSLvl</t>
-  </si>
-  <si>
-    <t>PeakTS</t>
-  </si>
-  <si>
-    <t>Ctype</t>
-  </si>
-  <si>
-    <t>Sets</t>
-  </si>
-  <si>
-    <t>EFF</t>
-  </si>
-  <si>
-    <t>~COMEMI</t>
-  </si>
-  <si>
-    <t>~FI_Process</t>
-  </si>
-  <si>
-    <t>Tact</t>
-  </si>
-  <si>
-    <t>Tcap</t>
-  </si>
-  <si>
-    <t>Tslvl</t>
-  </si>
-  <si>
-    <t>PrimaryCG</t>
-  </si>
-  <si>
-    <t>Vintage</t>
-  </si>
-  <si>
-    <t>\I: Commodity Set Membership</t>
-  </si>
-  <si>
-    <t>Commodity Name</t>
-  </si>
-  <si>
-    <t>Commodity Description</t>
-  </si>
-  <si>
-    <t>Balance Equ Type Override</t>
-  </si>
-  <si>
-    <t>Timeslice Tracking Level</t>
-  </si>
-  <si>
-    <t>Peak Monitoring</t>
-  </si>
-  <si>
-    <t>Electricity Indicator</t>
-  </si>
-  <si>
-    <t>\I: Process Set Membership</t>
-  </si>
-  <si>
-    <t>Technology Name</t>
-  </si>
-  <si>
-    <t>Technology Description</t>
-  </si>
-  <si>
-    <t>Activity Unit</t>
-  </si>
-  <si>
-    <t>Capacity Unit</t>
-  </si>
-  <si>
-    <t>Timeslice Operational Level</t>
-  </si>
-  <si>
-    <t>Operational Commodity Group</t>
-  </si>
-  <si>
-    <t>Vintage Tracking</t>
-  </si>
-  <si>
-    <t>&lt;Fuel Name&gt;</t>
-  </si>
-  <si>
-    <t>\I:Units</t>
-  </si>
-  <si>
-    <t>\I:Technology Name</t>
-  </si>
-  <si>
-    <t>Input Commodity</t>
-  </si>
-  <si>
-    <t>Output Commodity</t>
-  </si>
-  <si>
-    <t>Annual Availability Factor</t>
-  </si>
-  <si>
-    <t>Lifetime of Process</t>
-  </si>
-  <si>
-    <t>Capacity to Activity Factor</t>
-  </si>
-  <si>
-    <t>Starting Year</t>
-  </si>
-  <si>
-    <t>Investment Cost</t>
-  </si>
-  <si>
-    <t>Fixed O&amp;M Cost</t>
-  </si>
-  <si>
-    <t>Variable O&amp;M Cost</t>
-  </si>
-  <si>
-    <t>New Processes</t>
-  </si>
-  <si>
-    <t>*Declare and characterize the new technologies by sector. Sheet names should indicate the sector as &lt;SectorName&gt;_&lt;Anything&gt;</t>
-  </si>
-  <si>
-    <t>CURR</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>YEAR</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Availabity/Utilization Factor</t>
-  </si>
-  <si>
-    <t>NCAP_TLIFE</t>
-  </si>
-  <si>
-    <t>PRC_CAPACT</t>
-  </si>
-  <si>
-    <t>NCAP_AFA</t>
-  </si>
-  <si>
-    <t>NCAP_AF</t>
-  </si>
-  <si>
-    <t>NCAP_FOM</t>
-  </si>
-  <si>
-    <t>ACT_COST</t>
-  </si>
-  <si>
-    <t>NCAP_COST</t>
-  </si>
-  <si>
-    <t>Technical Efficiency</t>
-  </si>
-  <si>
-    <t>START</t>
-  </si>
-  <si>
-    <t>~PRCCOMEMI</t>
-  </si>
-  <si>
-    <t>NRG</t>
-  </si>
-  <si>
-    <t>ELCURN</t>
-  </si>
-  <si>
-    <t>Uranium ELC</t>
-  </si>
-  <si>
-    <t>PJ</t>
-  </si>
-  <si>
-    <t>ELCNGA</t>
-  </si>
-  <si>
-    <t>Natural Gas ELC</t>
-  </si>
-  <si>
-    <t>ELE</t>
-  </si>
-  <si>
-    <t>ETURNLWR13N</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>CHP</t>
-  </si>
-  <si>
-    <t>*Unit</t>
-  </si>
-  <si>
-    <t>Currency unit</t>
-  </si>
-  <si>
-    <t>Years</t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>ELCC</t>
-  </si>
-  <si>
-    <t>MEUR2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </t>
-  </si>
-  <si>
-    <t>MEUR2011</t>
-  </si>
-  <si>
-    <t>HET</t>
-  </si>
-  <si>
-    <t>M€/MW</t>
-  </si>
-  <si>
-    <t>M€/PJ</t>
-  </si>
-  <si>
-    <t>Lead Time between investment decision and actual availability of capacity (equal to construction time)</t>
-  </si>
-  <si>
-    <t>Fraction of capacity in peak equations</t>
-  </si>
-  <si>
-    <t>1/Cb: Ratio of heat produced to electricity produced</t>
-  </si>
-  <si>
-    <t>NCAP_ILED</t>
-  </si>
-  <si>
-    <t>NCAP_PKCNT</t>
-  </si>
-  <si>
-    <t>ECNGAGTBP15N</t>
-  </si>
-  <si>
-    <t>Thermal electric: Nuclear plant LWR (III Gen.) - Average size</t>
-  </si>
-  <si>
-    <t>ELCCO2</t>
-  </si>
-  <si>
-    <t>Kg/GJ</t>
-  </si>
-  <si>
-    <t>NCAP_CHPR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
@@ -1277,19 +1294,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1303,10 +1316,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1319,8 +1332,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1329,21 +1341,21 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 3" xfId="2"/>
-    <cellStyle name="Normale_B2020" xfId="3"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 10 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normale_B2020" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1359,7 +1371,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -1494,9 +1506,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1534,9 +1546,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1571,7 +1583,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1606,7 +1618,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1779,52 +1791,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="49.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" customWidth="1"/>
-    <col min="16" max="16" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.88671875" customWidth="1"/>
-    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.109375" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B2" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-    </row>
-    <row r="4" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
@@ -1832,12 +1844,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="2:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
-        <v>50</v>
+    <row r="6" spans="2:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
@@ -1845,729 +1857,729 @@
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" s="3" customFormat="1" ht="38.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7" s="12" t="s">
+      <c r="H8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="M7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" s="3" customFormat="1" ht="38.700000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="J8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="P8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="13" t="s">
+      <c r="Q8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="S8" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="U8"/>
       <c r="V8"/>
     </row>
-    <row r="9" spans="2:22" s="3" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="17" t="s">
+    <row r="9" spans="2:22" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="L9" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="N9" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="O9" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="R9" s="17" t="s">
+      <c r="P9" s="16"/>
+      <c r="Q9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="S9" s="17"/>
+      <c r="R9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="S9" s="15"/>
       <c r="U9"/>
       <c r="V9"/>
     </row>
-    <row r="10" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="19" t="s">
+    <row r="10" spans="2:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="17">
+        <v>2013</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="17">
+        <v>2013</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17">
+        <v>60</v>
+      </c>
+      <c r="L10" s="18">
+        <v>5.998310991957104</v>
+      </c>
+      <c r="M10" s="18">
+        <v>9.4473398123324406E-2</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0.6942489574024423</v>
+      </c>
+      <c r="O10" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="R10" s="17">
+        <v>6</v>
+      </c>
+      <c r="S10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="19">
+        <v>0.37</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="19">
+        <v>5.7983672922252012</v>
+      </c>
+      <c r="M11" s="19">
+        <v>9.1324284852546914E-2</v>
+      </c>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4">
+        <v>6</v>
+      </c>
+      <c r="S11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <v>2030</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="19">
+        <v>0.38</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="19">
+        <v>5.4484658176943705</v>
+      </c>
+      <c r="M12" s="19">
+        <v>7.7878071045576411E-2</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4">
+        <v>6</v>
+      </c>
+      <c r="S12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
+        <v>2040</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="19">
+        <v>0.38</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="19">
+        <v>5.0485784182305622</v>
+      </c>
+      <c r="M13" s="19">
+        <v>6.458181501340482E-2</v>
+      </c>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4">
+        <v>6</v>
+      </c>
+      <c r="S13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
+        <v>2050</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="19">
+        <v>0.38</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="19">
+        <v>4.9985924932975871</v>
+      </c>
+      <c r="M14" s="19">
+        <v>5.9983109919571044E-2</v>
+      </c>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4">
+        <v>6</v>
+      </c>
+      <c r="S14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="17">
+        <v>2015</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="17">
+        <v>2015</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="J15" s="18">
+        <v>1.0638297872340425</v>
+      </c>
+      <c r="K15" s="17">
+        <v>25</v>
+      </c>
+      <c r="L15" s="18">
+        <v>0.64912868632707776</v>
+      </c>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18">
+        <v>0.88769734882335394</v>
+      </c>
+      <c r="O15" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="R15" s="17">
+        <v>2</v>
+      </c>
+      <c r="S15" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="20">
+        <v>2020</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21">
+        <v>0.46</v>
+      </c>
+      <c r="J16" s="21">
+        <v>0.93457943925233644</v>
+      </c>
+      <c r="K16" s="20"/>
+      <c r="L16" s="21">
+        <v>0.59919571045576403</v>
+      </c>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21">
+        <v>0.94317843312481364</v>
+      </c>
+      <c r="O16" s="21"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="19">
-        <v>2013</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="19">
-        <v>2013</v>
-      </c>
-      <c r="I10" s="20">
-        <v>0.37</v>
-      </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19">
-        <v>60</v>
-      </c>
-      <c r="L10" s="20">
-        <v>5.998310991957104</v>
-      </c>
-      <c r="M10" s="20">
-        <v>9.4473398123324406E-2</v>
-      </c>
-      <c r="N10" s="20">
-        <v>0.6942489574024423</v>
-      </c>
-      <c r="O10" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="R10" s="19">
-        <v>6</v>
-      </c>
-      <c r="S10" s="19">
+      <c r="E22" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="27"/>
+      <c r="C23" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21">
-        <v>2020</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22">
-        <v>0.37</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="22">
-        <v>5.7983672922252012</v>
-      </c>
-      <c r="M11" s="22">
-        <v>9.1324284852546914E-2</v>
-      </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21">
-        <v>6</v>
-      </c>
-      <c r="S11" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21">
-        <v>2030</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22">
-        <v>0.38</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22">
-        <v>5.4484658176943705</v>
-      </c>
-      <c r="M12" s="22">
-        <v>7.7878071045576411E-2</v>
-      </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21">
-        <v>6</v>
-      </c>
-      <c r="S12" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21">
-        <v>2040</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="22">
-        <v>0.38</v>
-      </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="22">
-        <v>5.0485784182305622</v>
-      </c>
-      <c r="M13" s="22">
-        <v>6.458181501340482E-2</v>
-      </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21">
-        <v>6</v>
-      </c>
-      <c r="S13" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21">
-        <v>2050</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22">
-        <v>0.38</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="22">
-        <v>4.9985924932975871</v>
-      </c>
-      <c r="M14" s="22">
-        <v>5.9983109919571044E-2</v>
-      </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21">
-        <v>6</v>
-      </c>
-      <c r="S14" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="19">
-        <v>2015</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="19">
-        <v>2015</v>
-      </c>
-      <c r="I15" s="20">
-        <v>0.39500000000000002</v>
-      </c>
-      <c r="J15" s="20">
-        <v>1.0638297872340425</v>
-      </c>
-      <c r="K15" s="19">
-        <v>25</v>
-      </c>
-      <c r="L15" s="20">
-        <v>0.64912868632707776</v>
-      </c>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20">
-        <v>0.88769734882335394</v>
-      </c>
-      <c r="O15" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="R15" s="19">
-        <v>2</v>
-      </c>
-      <c r="S15" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="23">
-        <v>2020</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="24">
-        <v>0.46</v>
-      </c>
-      <c r="J16" s="24">
-        <v>0.93457943925233644</v>
-      </c>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24">
-        <v>0.59919571045576403</v>
-      </c>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24">
-        <v>0.94317843312481364</v>
-      </c>
-      <c r="O16" s="24"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="29" t="s">
+      <c r="D28" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="30"/>
-      <c r="C23" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="30" t="s">
+      <c r="C29" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="30" t="str">
+      <c r="C30" s="27" t="str">
         <f>B10</f>
         <v>ETURNLWR13N</v>
       </c>
-      <c r="D30" s="30" t="str">
+      <c r="D30" s="27" t="str">
         <f>C10</f>
         <v>Thermal electric: Nuclear plant LWR (III Gen.) - Average size</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="30" t="s">
+      <c r="E30" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30" t="s">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="30" t="str">
+      <c r="C31" s="27" t="str">
         <f>B15</f>
         <v>ECNGAGTBP15N</v>
       </c>
-      <c r="D31" s="30" t="str">
+      <c r="D31" s="27" t="str">
         <f>C15</f>
         <v xml:space="preserve">Gas Turbine Single Cycle - Large Scale Plant </v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="30" t="s">
+      <c r="E31" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="7"/>
+    </row>
+    <row r="34" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="11">
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="9">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="9" t="s">
+      <c r="C41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>